<commit_message>
watch the vote algo!
</commit_message>
<xml_diff>
--- a/Results-Lilim-100Nodes.xlsx
+++ b/Results-Lilim-100Nodes.xlsx
@@ -663,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AF7" sqref="AF7:AJ20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1757,14 +1757,43 @@
         <f t="shared" si="4"/>
         <v>24.363980674743537</v>
       </c>
-      <c r="Z7" s="2"/>
+      <c r="Z7">
+        <v>224.392720994386</v>
+      </c>
+      <c r="AA7">
+        <v>122.610342876516</v>
+      </c>
+      <c r="AB7">
+        <v>144.47355668633099</v>
+      </c>
+      <c r="AC7">
+        <v>194.86579477158401</v>
+      </c>
+      <c r="AD7">
+        <v>50.142135623730901</v>
+      </c>
       <c r="AE7" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>736.48455095254792</v>
+      </c>
+      <c r="AF7">
+        <v>6.4481133937835597</v>
+      </c>
+      <c r="AG7">
+        <v>5.1103742361068702</v>
+      </c>
+      <c r="AH7">
+        <v>5.1814262866973797</v>
+      </c>
+      <c r="AI7">
+        <v>11.501571488380399</v>
+      </c>
+      <c r="AJ7">
+        <v>1.30596985816955</v>
       </c>
       <c r="AK7" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>29.54745526313776</v>
       </c>
       <c r="AL7" s="2">
         <v>151.83723053454599</v>
@@ -1928,14 +1957,43 @@
         <f t="shared" si="4"/>
         <v>10.488498735427846</v>
       </c>
-      <c r="Z8" s="2"/>
+      <c r="Z8">
+        <v>142.46396047337799</v>
+      </c>
+      <c r="AA8">
+        <v>105.527478750375</v>
+      </c>
+      <c r="AB8">
+        <v>148.51835634154801</v>
+      </c>
+      <c r="AC8">
+        <v>197.958450110923</v>
+      </c>
+      <c r="AD8">
+        <v>52.527300430865402</v>
+      </c>
       <c r="AE8" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>646.99554610708935</v>
+      </c>
+      <c r="AF8">
+        <v>3.86283538341522</v>
+      </c>
+      <c r="AG8">
+        <v>2.4356332540511998</v>
+      </c>
+      <c r="AH8">
+        <v>2.6713542461395199</v>
+      </c>
+      <c r="AI8">
+        <v>5.1133911132812502</v>
+      </c>
+      <c r="AJ8">
+        <v>1.3428739786148001</v>
       </c>
       <c r="AK8" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>15.426087975501989</v>
       </c>
       <c r="AL8" s="2">
         <v>148.756384553087</v>
@@ -2099,37 +2157,81 @@
         <f t="shared" si="4"/>
         <v>11.123294472694379</v>
       </c>
-      <c r="Z9" s="2"/>
-      <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
-      <c r="AC9" s="3"/>
-      <c r="AD9" s="3"/>
+      <c r="Z9">
+        <v>204.67551133961501</v>
+      </c>
+      <c r="AA9">
+        <v>105.826733512215</v>
+      </c>
+      <c r="AB9">
+        <v>148.51835634154801</v>
+      </c>
+      <c r="AC9">
+        <v>269.12245973323201</v>
+      </c>
+      <c r="AD9">
+        <v>52.527300430865402</v>
+      </c>
       <c r="AE9" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AF9" s="2"/>
-      <c r="AG9" s="3"/>
-      <c r="AH9" s="3"/>
-      <c r="AI9" s="3"/>
-      <c r="AJ9" s="3"/>
+        <v>780.67036135747549</v>
+      </c>
+      <c r="AF9">
+        <v>3.8062079906463602</v>
+      </c>
+      <c r="AG9">
+        <v>2.1603329896926802</v>
+      </c>
+      <c r="AH9">
+        <v>3.1446794033050498</v>
+      </c>
+      <c r="AI9">
+        <v>6.1178484201431198</v>
+      </c>
+      <c r="AJ9">
+        <v>1.49938950538635</v>
+      </c>
       <c r="AK9" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AL9" s="2"/>
+        <v>16.728458309173561</v>
+      </c>
+      <c r="AL9" s="2">
+        <v>148.756384553087</v>
+      </c>
+      <c r="AM9">
+        <v>98.782327103466301</v>
+      </c>
+      <c r="AN9">
+        <v>148.51835634154801</v>
+      </c>
+      <c r="AO9">
+        <v>197.958450110923</v>
+      </c>
+      <c r="AP9">
+        <v>52.527300430865402</v>
+      </c>
       <c r="AQ9" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AR9" s="2"/>
-      <c r="AS9" s="3"/>
-      <c r="AT9" s="3"/>
-      <c r="AU9" s="3"/>
-      <c r="AV9" s="3"/>
+        <v>646.54281853988959</v>
+      </c>
+      <c r="AR9">
+        <v>5.6080579280853202</v>
+      </c>
+      <c r="AS9">
+        <v>2.8520595550537098</v>
+      </c>
+      <c r="AT9">
+        <v>3.4536405801773</v>
+      </c>
+      <c r="AU9">
+        <v>6.5061832427978503</v>
+      </c>
+      <c r="AV9">
+        <v>1.7566189050674399</v>
+      </c>
       <c r="AW9" s="3">
         <f t="shared" ref="AW9:AW48" si="10">SUM(AR9:AV9)</f>
-        <v>0</v>
+        <v>20.17656021118162</v>
       </c>
       <c r="AX9" s="2">
         <v>159.20070889874299</v>
@@ -2255,33 +2357,81 @@
         <f t="shared" si="4"/>
         <v>11.147950792312608</v>
       </c>
-      <c r="Z10" s="2"/>
+      <c r="Z10">
+        <v>110.206699026359</v>
+      </c>
+      <c r="AA10">
+        <v>110.50607510501101</v>
+      </c>
+      <c r="AB10">
+        <v>148.51835634154801</v>
+      </c>
+      <c r="AC10">
+        <v>201.14593791939001</v>
+      </c>
+      <c r="AD10">
+        <v>52.527300430865402</v>
+      </c>
       <c r="AE10" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AF10" s="2"/>
-      <c r="AG10" s="3"/>
-      <c r="AH10" s="3"/>
-      <c r="AI10" s="3"/>
-      <c r="AJ10" s="3"/>
+        <v>622.9043688231734</v>
+      </c>
+      <c r="AF10">
+        <v>3.7380420923233002</v>
+      </c>
+      <c r="AG10">
+        <v>3.0149364471435498</v>
+      </c>
+      <c r="AH10">
+        <v>3.0847069025039602</v>
+      </c>
+      <c r="AI10">
+        <v>5.7658711671829197</v>
+      </c>
+      <c r="AJ10">
+        <v>1.4546997785568201</v>
+      </c>
       <c r="AK10" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AL10" s="2"/>
+        <v>17.05825638771055</v>
+      </c>
+      <c r="AL10" s="2">
+        <v>145.304880483967</v>
+      </c>
+      <c r="AM10">
+        <v>105.82271429207501</v>
+      </c>
+      <c r="AN10">
+        <v>148.51835634154801</v>
+      </c>
+      <c r="AO10">
+        <v>201.14593791939001</v>
+      </c>
+      <c r="AP10">
+        <v>52.527300430865402</v>
+      </c>
       <c r="AQ10" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AR10" s="2"/>
-      <c r="AS10" s="3"/>
-      <c r="AT10" s="3"/>
-      <c r="AU10" s="3"/>
-      <c r="AV10" s="3"/>
+        <v>653.31918946784538</v>
+      </c>
+      <c r="AR10">
+        <v>5.0593881130218499</v>
+      </c>
+      <c r="AS10">
+        <v>2.9896446466445901</v>
+      </c>
+      <c r="AT10">
+        <v>3.95691270828247</v>
+      </c>
+      <c r="AU10">
+        <v>6.6442367792129504</v>
+      </c>
+      <c r="AV10">
+        <v>1.88884816169738</v>
+      </c>
       <c r="AW10" s="3">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>20.53903040885924</v>
       </c>
       <c r="AX10" s="2">
         <v>147.69962901947</v>
@@ -2407,28 +2557,81 @@
         <f t="shared" si="4"/>
         <v>13.3904538631439</v>
       </c>
-      <c r="Z11" s="2"/>
+      <c r="Z11">
+        <v>110.206699026359</v>
+      </c>
+      <c r="AA11">
+        <v>110.40725555812899</v>
+      </c>
+      <c r="AB11">
+        <v>148.51835634154801</v>
+      </c>
+      <c r="AC11">
+        <v>201.212942557161</v>
+      </c>
+      <c r="AD11">
+        <v>52.527300430865402</v>
+      </c>
       <c r="AE11" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AF11" s="2"/>
-      <c r="AG11" s="3"/>
-      <c r="AH11" s="3"/>
-      <c r="AI11" s="3"/>
-      <c r="AJ11" s="3"/>
+        <v>622.87255391406234</v>
+      </c>
+      <c r="AF11">
+        <v>4.2778151273727403</v>
+      </c>
+      <c r="AG11">
+        <v>2.9406144380569401</v>
+      </c>
+      <c r="AH11">
+        <v>3.2724629878997802</v>
+      </c>
+      <c r="AI11">
+        <v>6.5292543172836304</v>
+      </c>
+      <c r="AJ11">
+        <v>1.58541121482849</v>
+      </c>
       <c r="AK11" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AL11" s="2"/>
+        <v>18.605558085441579</v>
+      </c>
+      <c r="AL11" s="2">
+        <v>156.40896749275601</v>
+      </c>
+      <c r="AM11">
+        <v>96.490641965189297</v>
+      </c>
+      <c r="AN11">
+        <v>148.51835634154801</v>
+      </c>
+      <c r="AO11">
+        <v>201.14593791939001</v>
+      </c>
+      <c r="AP11">
+        <v>52.527300430865402</v>
+      </c>
       <c r="AQ11" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>655.09120414974871</v>
+      </c>
+      <c r="AR11">
+        <v>6.1351145744323698</v>
+      </c>
+      <c r="AS11">
+        <v>2.8313804864883401</v>
+      </c>
+      <c r="AT11">
+        <v>3.5628847122192302</v>
+      </c>
+      <c r="AU11">
+        <v>6.6748054027557302</v>
+      </c>
+      <c r="AV11">
+        <v>1.67352073192596</v>
       </c>
       <c r="AW11" s="3">
         <f>SUM(AR11:AV11)</f>
-        <v>0</v>
+        <v>20.877705907821632</v>
       </c>
       <c r="AX11" s="2">
         <v>151.98178517246799</v>
@@ -2554,28 +2757,81 @@
         <f t="shared" si="4"/>
         <v>21.886188673973063</v>
       </c>
-      <c r="Z12" s="2"/>
+      <c r="Z12">
+        <v>161.70065646308601</v>
+      </c>
+      <c r="AA12">
+        <v>80.416179041571795</v>
+      </c>
+      <c r="AB12">
+        <v>148.51835634154801</v>
+      </c>
+      <c r="AC12">
+        <v>201.14593791939001</v>
+      </c>
+      <c r="AD12">
+        <v>52.527300430865402</v>
+      </c>
       <c r="AE12" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AF12" s="2"/>
-      <c r="AG12" s="3"/>
-      <c r="AH12" s="3"/>
-      <c r="AI12" s="3"/>
-      <c r="AJ12" s="3"/>
+        <v>644.30843019646113</v>
+      </c>
+      <c r="AF12">
+        <v>11.5257639884948</v>
+      </c>
+      <c r="AG12">
+        <v>2.2050282239913899</v>
+      </c>
+      <c r="AH12">
+        <v>4.90048344135284</v>
+      </c>
+      <c r="AI12">
+        <v>8.5598953723907396</v>
+      </c>
+      <c r="AJ12">
+        <v>1.69239401817321</v>
+      </c>
       <c r="AK12" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AL12" s="2"/>
+        <v>28.883565044402978</v>
+      </c>
+      <c r="AL12" s="2">
+        <v>151.98178517246799</v>
+      </c>
+      <c r="AM12">
+        <v>96.589732841017593</v>
+      </c>
+      <c r="AN12">
+        <v>148.51835634154801</v>
+      </c>
+      <c r="AO12">
+        <v>201.27994719493199</v>
+      </c>
+      <c r="AP12">
+        <v>52.527300430865402</v>
+      </c>
       <c r="AQ12" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>650.89712198083089</v>
+      </c>
+      <c r="AR12">
+        <v>6.8331749677657996</v>
+      </c>
+      <c r="AS12">
+        <v>3.08958451747894</v>
+      </c>
+      <c r="AT12">
+        <v>4.01715061664581</v>
+      </c>
+      <c r="AU12">
+        <v>8.6047090530395494</v>
+      </c>
+      <c r="AV12">
+        <v>1.9274831056594799</v>
       </c>
       <c r="AW12" s="3">
         <f>SUM(AR12:AV12)</f>
-        <v>0</v>
+        <v>24.47210226058958</v>
       </c>
       <c r="AX12" s="2">
         <v>159.53160835793099</v>
@@ -2701,28 +2957,81 @@
         <f t="shared" si="4"/>
         <v>12.453018999099708</v>
       </c>
-      <c r="Z13" s="2"/>
+      <c r="Z13">
+        <v>155.07506374327701</v>
+      </c>
+      <c r="AA13">
+        <v>152.765610009699</v>
+      </c>
+      <c r="AB13">
+        <v>238.63534163309501</v>
+      </c>
+      <c r="AC13">
+        <v>284.08022337934</v>
+      </c>
+      <c r="AD13">
+        <v>109.154249735316</v>
+      </c>
       <c r="AE13" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AF13" s="2"/>
-      <c r="AG13" s="3"/>
-      <c r="AH13" s="3"/>
-      <c r="AI13" s="3"/>
-      <c r="AJ13" s="3"/>
+        <v>939.71048850072702</v>
+      </c>
+      <c r="AF13">
+        <v>1.87750022411346</v>
+      </c>
+      <c r="AG13">
+        <v>2.5129470109939498</v>
+      </c>
+      <c r="AH13">
+        <v>4.0443292856216404</v>
+      </c>
+      <c r="AI13">
+        <v>8.4266450166702196</v>
+      </c>
+      <c r="AJ13">
+        <v>0.87984113693237298</v>
+      </c>
       <c r="AK13" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AL13" s="2"/>
+        <v>17.741262674331644</v>
+      </c>
+      <c r="AL13" s="2">
+        <v>159.53160835793099</v>
+      </c>
+      <c r="AM13">
+        <v>80.416179041571795</v>
+      </c>
+      <c r="AN13">
+        <v>148.51835634154801</v>
+      </c>
+      <c r="AO13">
+        <v>201.14593791939001</v>
+      </c>
+      <c r="AP13">
+        <v>97.6493571215793</v>
+      </c>
       <c r="AQ13" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>687.26143878202015</v>
+      </c>
+      <c r="AR13">
+        <v>11.1501729011535</v>
+      </c>
+      <c r="AS13">
+        <v>2.58296480178833</v>
+      </c>
+      <c r="AT13">
+        <v>5.8834872961044304</v>
+      </c>
+      <c r="AU13">
+        <v>10.800409221649099</v>
+      </c>
+      <c r="AV13">
+        <v>2.5140008449554401</v>
       </c>
       <c r="AW13" s="3">
         <f>SUM(AR13:AV13)</f>
-        <v>0</v>
+        <v>32.931035065650796</v>
       </c>
       <c r="AX13" s="2">
         <v>191.60109661909999</v>
@@ -2854,32 +3163,81 @@
         <f t="shared" si="4"/>
         <v>17.789727473258949</v>
       </c>
-      <c r="Z14" s="2"/>
+      <c r="Z14">
+        <v>193.82017561776101</v>
+      </c>
+      <c r="AA14">
+        <v>194.841703421321</v>
+      </c>
+      <c r="AB14">
+        <v>203.28513804065699</v>
+      </c>
+      <c r="AC14">
+        <v>179.94992639992799</v>
+      </c>
+      <c r="AD14">
+        <v>170.677305023836</v>
+      </c>
       <c r="AE14" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AF14" s="2"/>
-      <c r="AG14" s="3"/>
-      <c r="AH14" s="3"/>
-      <c r="AI14" s="3"/>
-      <c r="AJ14" s="3"/>
+        <v>942.57424850350299</v>
+      </c>
+      <c r="AF14">
+        <v>1.9990540981292699</v>
+      </c>
+      <c r="AG14">
+        <v>8.3612008571624692</v>
+      </c>
+      <c r="AH14">
+        <v>7.2377205610275199</v>
+      </c>
+      <c r="AI14">
+        <v>9.5814216613769503</v>
+      </c>
+      <c r="AJ14">
+        <v>3.1608600139617899</v>
+      </c>
       <c r="AK14" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AL14" s="2"/>
-      <c r="AM14" s="3"/>
-      <c r="AN14" s="3"/>
-      <c r="AO14" s="3"/>
-      <c r="AP14" s="3"/>
+        <v>30.340257191658001</v>
+      </c>
+      <c r="AL14" s="2">
+        <v>251.68529934636101</v>
+      </c>
+      <c r="AM14">
+        <v>152.765610009699</v>
+      </c>
+      <c r="AN14">
+        <v>236.49151882785301</v>
+      </c>
+      <c r="AO14">
+        <v>255.51866651167501</v>
+      </c>
+      <c r="AP14">
+        <v>147.44960822020801</v>
+      </c>
       <c r="AQ14" s="5">
-        <f t="shared" ref="AQ10:AQ48" si="11">SUM(AL14:AP14)</f>
-        <v>0</v>
+        <f t="shared" ref="AQ14:AQ48" si="11">SUM(AL14:AP14)</f>
+        <v>1043.9107029157963</v>
+      </c>
+      <c r="AR14">
+        <v>4.2835056543350198</v>
+      </c>
+      <c r="AS14">
+        <v>3.27147009372711</v>
+      </c>
+      <c r="AT14">
+        <v>4.4375966548919603</v>
+      </c>
+      <c r="AU14">
+        <v>8.2360730409622196</v>
+      </c>
+      <c r="AV14">
+        <v>1.38465197086334</v>
       </c>
       <c r="AW14" s="3">
         <f>SUM(AR14:AV14)</f>
-        <v>0</v>
+        <v>21.613297414779652</v>
       </c>
       <c r="AX14" s="2">
         <v>162.23528861629501</v>
@@ -3011,36 +3369,81 @@
         <f t="shared" si="4"/>
         <v>33.008878064155539</v>
       </c>
-      <c r="Z15" s="2"/>
-      <c r="AA15" s="3"/>
-      <c r="AB15" s="3"/>
-      <c r="AC15" s="3"/>
-      <c r="AD15" s="3"/>
+      <c r="Z15">
+        <v>216.88338867046099</v>
+      </c>
+      <c r="AA15">
+        <v>179.98771894786299</v>
+      </c>
+      <c r="AB15">
+        <v>193.72975940217401</v>
+      </c>
+      <c r="AC15">
+        <v>156.713295910813</v>
+      </c>
+      <c r="AD15">
+        <v>168.49066569943801</v>
+      </c>
       <c r="AE15" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AF15" s="2"/>
-      <c r="AG15" s="3"/>
-      <c r="AH15" s="3"/>
-      <c r="AI15" s="3"/>
-      <c r="AJ15" s="3"/>
+        <v>915.80482863074917</v>
+      </c>
+      <c r="AF15">
+        <v>4.2612520694732599</v>
+      </c>
+      <c r="AG15">
+        <v>9.7526063203811599</v>
+      </c>
+      <c r="AH15">
+        <v>8.1418722391128497</v>
+      </c>
+      <c r="AI15">
+        <v>14.217589473724299</v>
+      </c>
+      <c r="AJ15">
+        <v>4.4080167770385703</v>
+      </c>
       <c r="AK15" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AL15" s="2"/>
-      <c r="AM15" s="3"/>
-      <c r="AN15" s="3"/>
-      <c r="AO15" s="3"/>
-      <c r="AP15" s="3"/>
+        <v>40.781336879730134</v>
+      </c>
+      <c r="AL15" s="2">
+        <v>327.04614536947798</v>
+      </c>
+      <c r="AM15">
+        <v>169.55286584768399</v>
+      </c>
+      <c r="AN15">
+        <v>175.027007071204</v>
+      </c>
+      <c r="AO15">
+        <v>273.39826674909801</v>
+      </c>
+      <c r="AP15">
+        <v>203.96616199574001</v>
+      </c>
       <c r="AQ15" s="5">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1148.9904470332042</v>
+      </c>
+      <c r="AR15">
+        <v>6.8256854534149101</v>
+      </c>
+      <c r="AS15">
+        <v>2.9797410964965798</v>
+      </c>
+      <c r="AT15">
+        <v>4.0920321941375697</v>
+      </c>
+      <c r="AU15">
+        <v>13.5486724138259</v>
+      </c>
+      <c r="AV15">
+        <v>4.9146657943725502</v>
       </c>
       <c r="AW15" s="3">
         <f>SUM(AR15:AV15)</f>
-        <v>0</v>
+        <v>32.360796952247512</v>
       </c>
       <c r="AX15" s="2">
         <v>154.15981694475701</v>
@@ -3172,41 +3575,81 @@
         <f t="shared" si="4"/>
         <v>68.697053098678566</v>
       </c>
-      <c r="Z16" s="2"/>
-      <c r="AA16" s="3"/>
-      <c r="AB16" s="3"/>
-      <c r="AC16" s="3"/>
-      <c r="AD16" s="3"/>
+      <c r="Z16">
+        <v>209.47544395263799</v>
+      </c>
+      <c r="AA16">
+        <v>122.70776287405</v>
+      </c>
+      <c r="AB16">
+        <v>211.580823918362</v>
+      </c>
+      <c r="AC16">
+        <v>274.810707801825</v>
+      </c>
+      <c r="AD16">
+        <v>155.22345769943701</v>
+      </c>
       <c r="AE16" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AF16" s="2"/>
-      <c r="AG16" s="3"/>
-      <c r="AH16" s="3"/>
-      <c r="AI16" s="3"/>
-      <c r="AJ16" s="3"/>
+        <v>973.79819624631182</v>
+      </c>
+      <c r="AF16">
+        <v>9.5542085409164397</v>
+      </c>
+      <c r="AG16">
+        <v>5.3604382038116398</v>
+      </c>
+      <c r="AH16">
+        <v>11.6110980987548</v>
+      </c>
+      <c r="AI16">
+        <v>52.129576182365398</v>
+      </c>
+      <c r="AJ16">
+        <v>2.4396843433380102</v>
+      </c>
       <c r="AK16" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AL16" s="2"/>
-      <c r="AM16" s="3"/>
-      <c r="AN16" s="3"/>
-      <c r="AO16" s="3"/>
-      <c r="AP16" s="3"/>
+        <v>81.095005369186296</v>
+      </c>
+      <c r="AL16" s="2">
+        <v>227.96857450015699</v>
+      </c>
+      <c r="AM16">
+        <v>179.98771894786299</v>
+      </c>
+      <c r="AN16">
+        <v>169.836294051935</v>
+      </c>
+      <c r="AO16">
+        <v>259.562654676779</v>
+      </c>
+      <c r="AP16">
+        <v>203.96616199574001</v>
+      </c>
       <c r="AQ16" s="5">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AR16" s="2"/>
-      <c r="AS16" s="3"/>
-      <c r="AT16" s="3"/>
-      <c r="AU16" s="3"/>
-      <c r="AV16" s="3"/>
+        <v>1041.3214041724741</v>
+      </c>
+      <c r="AR16">
+        <v>3.4398366689682001</v>
+      </c>
+      <c r="AS16">
+        <v>11.8569980382919</v>
+      </c>
+      <c r="AT16">
+        <v>4.9848235845565796</v>
+      </c>
+      <c r="AU16">
+        <v>24.060271906852702</v>
+      </c>
+      <c r="AV16">
+        <v>6.6328755140304496</v>
+      </c>
       <c r="AW16" s="3">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>50.974805712699833</v>
       </c>
       <c r="AX16" s="2">
         <v>209.47544395263799</v>
@@ -3338,41 +3781,81 @@
         <f t="shared" si="4"/>
         <v>18.788391184806802</v>
       </c>
-      <c r="Z17" s="2"/>
-      <c r="AA17" s="3"/>
-      <c r="AB17" s="3"/>
-      <c r="AC17" s="3"/>
-      <c r="AD17" s="3"/>
+      <c r="Z17">
+        <v>255.03155596785001</v>
+      </c>
+      <c r="AA17">
+        <v>153.274802852101</v>
+      </c>
+      <c r="AB17">
+        <v>201.234408199353</v>
+      </c>
+      <c r="AC17">
+        <v>217.77063368948899</v>
+      </c>
+      <c r="AD17">
+        <v>152.961126160129</v>
+      </c>
       <c r="AE17" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AF17" s="2"/>
-      <c r="AG17" s="3"/>
-      <c r="AH17" s="3"/>
-      <c r="AI17" s="3"/>
-      <c r="AJ17" s="3"/>
+        <v>980.27252686892189</v>
+      </c>
+      <c r="AF17">
+        <v>5.2015434265136697</v>
+      </c>
+      <c r="AG17">
+        <v>4.9281017541885301</v>
+      </c>
+      <c r="AH17">
+        <v>4.5681679487228397</v>
+      </c>
+      <c r="AI17">
+        <v>5.7508327245712199</v>
+      </c>
+      <c r="AJ17">
+        <v>2.0483695030212399</v>
+      </c>
       <c r="AK17" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AL17" s="2"/>
-      <c r="AM17" s="3"/>
-      <c r="AN17" s="3"/>
-      <c r="AO17" s="3"/>
-      <c r="AP17" s="3"/>
+        <v>22.497015357017503</v>
+      </c>
+      <c r="AL17" s="2">
+        <v>227.55330022553099</v>
+      </c>
+      <c r="AM17">
+        <v>151.758552352408</v>
+      </c>
+      <c r="AN17">
+        <v>134.84679129158599</v>
+      </c>
+      <c r="AO17">
+        <v>255.33792632727699</v>
+      </c>
+      <c r="AP17">
+        <v>203.35855179665899</v>
+      </c>
       <c r="AQ17" s="5">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AR17" s="2"/>
-      <c r="AS17" s="3"/>
-      <c r="AT17" s="3"/>
-      <c r="AU17" s="3"/>
-      <c r="AV17" s="3"/>
+        <v>972.8551219934609</v>
+      </c>
+      <c r="AR17">
+        <v>7.6492364168167102</v>
+      </c>
+      <c r="AS17">
+        <v>7.71581628322601</v>
+      </c>
+      <c r="AT17">
+        <v>6.24365134239196</v>
+      </c>
+      <c r="AU17">
+        <v>72.714664030074999</v>
+      </c>
+      <c r="AV17">
+        <v>6.0432926177978503</v>
+      </c>
       <c r="AW17" s="3">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>100.36666069030753</v>
       </c>
       <c r="AX17" s="2">
         <v>255.03155596785001</v>
@@ -3504,41 +3987,81 @@
         <f t="shared" si="4"/>
         <v>32.700722789764278</v>
       </c>
-      <c r="Z18" s="2"/>
-      <c r="AA18" s="3"/>
-      <c r="AB18" s="3"/>
-      <c r="AC18" s="3"/>
-      <c r="AD18" s="3"/>
+      <c r="Z18">
+        <v>85.3842548474681</v>
+      </c>
+      <c r="AA18">
+        <v>139.64886821887001</v>
+      </c>
+      <c r="AB18">
+        <v>266.15681425643697</v>
+      </c>
+      <c r="AC18">
+        <v>320.72189039378702</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
       <c r="AE18" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AF18" s="2"/>
-      <c r="AG18" s="3"/>
-      <c r="AH18" s="3"/>
-      <c r="AI18" s="3"/>
-      <c r="AJ18" s="3"/>
+        <v>811.91182771656213</v>
+      </c>
+      <c r="AF18">
+        <v>1.2165066480636499</v>
+      </c>
+      <c r="AG18">
+        <v>2.53107237815856</v>
+      </c>
+      <c r="AH18">
+        <v>18.420865416526699</v>
+      </c>
+      <c r="AI18">
+        <v>20.141511464118899</v>
+      </c>
+      <c r="AJ18">
+        <v>0</v>
+      </c>
       <c r="AK18" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AL18" s="2"/>
-      <c r="AM18" s="3"/>
-      <c r="AN18" s="3"/>
-      <c r="AO18" s="3"/>
-      <c r="AP18" s="3"/>
+        <v>42.309955906867806</v>
+      </c>
+      <c r="AL18" s="2">
+        <v>313.13217148424201</v>
+      </c>
+      <c r="AM18">
+        <v>153.274802852101</v>
+      </c>
+      <c r="AN18">
+        <v>241.67154979377401</v>
+      </c>
+      <c r="AO18">
+        <v>186.905239211657</v>
+      </c>
+      <c r="AP18">
+        <v>115.566897157905</v>
+      </c>
       <c r="AQ18" s="5">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AR18" s="2"/>
-      <c r="AS18" s="3"/>
-      <c r="AT18" s="3"/>
-      <c r="AU18" s="3"/>
-      <c r="AV18" s="3"/>
+        <v>1010.550660499679</v>
+      </c>
+      <c r="AR18">
+        <v>7.0109284639358496</v>
+      </c>
+      <c r="AS18">
+        <v>5.9533527612686097</v>
+      </c>
+      <c r="AT18">
+        <v>7.8372111082076996</v>
+      </c>
+      <c r="AU18">
+        <v>6.4656742334365802</v>
+      </c>
+      <c r="AV18">
+        <v>1.9279176712036099</v>
+      </c>
       <c r="AW18" s="3">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>29.195084238052349</v>
       </c>
       <c r="AX18" s="2">
         <v>121.91028772329101</v>
@@ -3670,41 +4193,81 @@
         <f t="shared" si="4"/>
         <v>29.109723663330016</v>
       </c>
-      <c r="Z19" s="2"/>
-      <c r="AA19" s="3"/>
-      <c r="AB19" s="3"/>
-      <c r="AC19" s="3"/>
-      <c r="AD19" s="3"/>
+      <c r="Z19">
+        <v>171.64341002549</v>
+      </c>
+      <c r="AA19">
+        <v>153.06827551576001</v>
+      </c>
+      <c r="AB19">
+        <v>245.98456547815201</v>
+      </c>
+      <c r="AC19">
+        <v>234.51523448165599</v>
+      </c>
+      <c r="AD19">
+        <v>115.566897157905</v>
+      </c>
       <c r="AE19" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AF19" s="2"/>
-      <c r="AG19" s="3"/>
-      <c r="AH19" s="3"/>
-      <c r="AI19" s="3"/>
-      <c r="AJ19" s="3"/>
+        <v>920.77838265896298</v>
+      </c>
+      <c r="AF19">
+        <v>4.0760778427124</v>
+      </c>
+      <c r="AG19">
+        <v>11.0831034898757</v>
+      </c>
+      <c r="AH19">
+        <v>6.1199695110321004</v>
+      </c>
+      <c r="AI19">
+        <v>11.8077323198318</v>
+      </c>
+      <c r="AJ19">
+        <v>1.81134812831878</v>
+      </c>
       <c r="AK19" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AL19" s="2"/>
-      <c r="AM19" s="3"/>
-      <c r="AN19" s="3"/>
-      <c r="AO19" s="3"/>
-      <c r="AP19" s="3"/>
+        <v>34.898231291770777</v>
+      </c>
+      <c r="AL19" s="2">
+        <v>133.592581412154</v>
+      </c>
+      <c r="AM19">
+        <v>151.692810330192</v>
+      </c>
+      <c r="AN19">
+        <v>255.510506326995</v>
+      </c>
+      <c r="AO19">
+        <v>281.20181840403001</v>
+      </c>
+      <c r="AP19">
+        <v>71.054083775364404</v>
+      </c>
       <c r="AQ19" s="5">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AR19" s="2"/>
-      <c r="AS19" s="3"/>
-      <c r="AT19" s="3"/>
-      <c r="AU19" s="3"/>
-      <c r="AV19" s="3"/>
+        <v>893.05180024873539</v>
+      </c>
+      <c r="AR19">
+        <v>2.5208499908447202</v>
+      </c>
+      <c r="AS19">
+        <v>3.97108952999114</v>
+      </c>
+      <c r="AT19">
+        <v>16.043842387199401</v>
+      </c>
+      <c r="AU19">
+        <v>21.544659423828101</v>
+      </c>
+      <c r="AV19">
+        <v>0.87547054290771398</v>
+      </c>
       <c r="AW19" s="3">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>44.955911874771076</v>
       </c>
       <c r="AX19" s="2">
         <v>171.64341002549</v>
@@ -3836,41 +4399,81 @@
         <f t="shared" si="4"/>
         <v>29.494111752510037</v>
       </c>
-      <c r="Z20" s="2"/>
-      <c r="AA20" s="3"/>
-      <c r="AB20" s="3"/>
-      <c r="AC20" s="3"/>
-      <c r="AD20" s="3"/>
+      <c r="Z20">
+        <v>255.03155596785001</v>
+      </c>
+      <c r="AA20">
+        <v>153.10575474694599</v>
+      </c>
+      <c r="AB20">
+        <v>201.234408199353</v>
+      </c>
+      <c r="AC20">
+        <v>215.15452526107899</v>
+      </c>
+      <c r="AD20">
+        <v>152.961126160129</v>
+      </c>
       <c r="AE20" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AF20" s="2"/>
-      <c r="AG20" s="3"/>
-      <c r="AH20" s="3"/>
-      <c r="AI20" s="3"/>
-      <c r="AJ20" s="3"/>
+        <v>977.48737033535701</v>
+      </c>
+      <c r="AF20">
+        <v>8.1959123373031595</v>
+      </c>
+      <c r="AG20">
+        <v>6.7445632457733096</v>
+      </c>
+      <c r="AH20">
+        <v>6.7998101949691696</v>
+      </c>
+      <c r="AI20">
+        <v>10.5320385217666</v>
+      </c>
+      <c r="AJ20">
+        <v>2.71984872817993</v>
+      </c>
       <c r="AK20" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AL20" s="2"/>
-      <c r="AM20" s="3"/>
-      <c r="AN20" s="3"/>
-      <c r="AO20" s="3"/>
-      <c r="AP20" s="3"/>
+        <v>34.992173027992173</v>
+      </c>
+      <c r="AL20" s="2">
+        <v>264.96739219015802</v>
+      </c>
+      <c r="AM20">
+        <v>153.06827551576001</v>
+      </c>
+      <c r="AN20">
+        <v>241.723470577923</v>
+      </c>
+      <c r="AO20">
+        <v>215.15452526107899</v>
+      </c>
+      <c r="AP20">
+        <v>115.566897157905</v>
+      </c>
       <c r="AQ20" s="5">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AR20" s="2"/>
-      <c r="AS20" s="3"/>
-      <c r="AT20" s="3"/>
-      <c r="AU20" s="3"/>
-      <c r="AV20" s="3"/>
+        <v>990.48056070282507</v>
+      </c>
+      <c r="AR20">
+        <v>5.4499543905258099</v>
+      </c>
+      <c r="AS20">
+        <v>13.143904638290399</v>
+      </c>
+      <c r="AT20">
+        <v>6.0677769184112504</v>
+      </c>
+      <c r="AU20">
+        <v>12.1869487524032</v>
+      </c>
+      <c r="AV20">
+        <v>2.1155869722366298</v>
+      </c>
       <c r="AW20" s="3">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>38.964171671867291</v>
       </c>
       <c r="AX20" s="2">
         <v>255.03155596785001</v>
@@ -4020,23 +4623,43 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AL21" s="2"/>
-      <c r="AM21" s="3"/>
-      <c r="AN21" s="3"/>
-      <c r="AO21" s="3"/>
-      <c r="AP21" s="3"/>
+      <c r="AL21" s="2">
+        <v>228.99933861109699</v>
+      </c>
+      <c r="AM21">
+        <v>153.10575474694599</v>
+      </c>
+      <c r="AN21">
+        <v>245.93264469400401</v>
+      </c>
+      <c r="AO21">
+        <v>197.642056920106</v>
+      </c>
+      <c r="AP21">
+        <v>107.984927868296</v>
+      </c>
       <c r="AQ21" s="5">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AR21" s="2"/>
-      <c r="AS21" s="3"/>
-      <c r="AT21" s="3"/>
-      <c r="AU21" s="3"/>
-      <c r="AV21" s="3"/>
+        <v>933.66472284044903</v>
+      </c>
+      <c r="AR21">
+        <v>7.1176210403442299</v>
+      </c>
+      <c r="AS21">
+        <v>7.79207320213317</v>
+      </c>
+      <c r="AT21">
+        <v>15.0675921916961</v>
+      </c>
+      <c r="AU21">
+        <v>10.7663640022277</v>
+      </c>
+      <c r="AV21">
+        <v>2.3410719156265198</v>
+      </c>
       <c r="AW21" s="3">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>43.084722352027718</v>
       </c>
       <c r="AX21" s="2"/>
       <c r="AY21" s="3"/>
@@ -4166,23 +4789,43 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AL22" s="2"/>
-      <c r="AM22" s="3"/>
-      <c r="AN22" s="3"/>
-      <c r="AO22" s="3"/>
-      <c r="AP22" s="3"/>
+      <c r="AL22" s="2">
+        <v>327.04614536947798</v>
+      </c>
+      <c r="AM22">
+        <v>169.55286584768399</v>
+      </c>
+      <c r="AN22">
+        <v>175.027007071204</v>
+      </c>
+      <c r="AO22">
+        <v>273.39826674909801</v>
+      </c>
+      <c r="AP22">
+        <v>203.96616199574001</v>
+      </c>
       <c r="AQ22" s="5">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AR22" s="2"/>
-      <c r="AS22" s="3"/>
-      <c r="AT22" s="3"/>
-      <c r="AU22" s="3"/>
-      <c r="AV22" s="3"/>
+        <v>1148.9904470332042</v>
+      </c>
+      <c r="AR22">
+        <v>6.5207791805267297</v>
+      </c>
+      <c r="AS22">
+        <v>2.6828076839446999</v>
+      </c>
+      <c r="AT22">
+        <v>3.6186709165573099</v>
+      </c>
+      <c r="AU22">
+        <v>12.7025416851043</v>
+      </c>
+      <c r="AV22">
+        <v>4.40791537761688</v>
+      </c>
       <c r="AW22" s="3">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>29.93271484374992</v>
       </c>
       <c r="AX22" s="2"/>
       <c r="AY22" s="3"/>
@@ -4312,23 +4955,43 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AL23" s="2"/>
-      <c r="AM23" s="3"/>
-      <c r="AN23" s="3"/>
-      <c r="AO23" s="3"/>
-      <c r="AP23" s="3"/>
+      <c r="AL23" s="2">
+        <v>227.96857450015699</v>
+      </c>
+      <c r="AM23">
+        <v>179.98771894786299</v>
+      </c>
+      <c r="AN23">
+        <v>169.836294051935</v>
+      </c>
+      <c r="AO23">
+        <v>259.81692553721899</v>
+      </c>
+      <c r="AP23">
+        <v>203.96616199574001</v>
+      </c>
       <c r="AQ23" s="5">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AR23" s="2"/>
-      <c r="AS23" s="3"/>
-      <c r="AT23" s="3"/>
-      <c r="AU23" s="3"/>
-      <c r="AV23" s="3"/>
+        <v>1041.5756750329142</v>
+      </c>
+      <c r="AR23">
+        <v>3.5133681058883601</v>
+      </c>
+      <c r="AS23">
+        <v>11.807006478309599</v>
+      </c>
+      <c r="AT23">
+        <v>5.0805748462676998</v>
+      </c>
+      <c r="AU23">
+        <v>23.100161433219899</v>
+      </c>
+      <c r="AV23">
+        <v>6.7234407424926701</v>
+      </c>
       <c r="AW23" s="3">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>50.224551606178224</v>
       </c>
       <c r="AX23" s="2"/>
       <c r="AY23" s="3"/>
@@ -4458,23 +5121,43 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AL24" s="2"/>
-      <c r="AM24" s="3"/>
-      <c r="AN24" s="3"/>
-      <c r="AO24" s="3"/>
-      <c r="AP24" s="3"/>
+      <c r="AL24" s="2">
+        <v>227.49370614343701</v>
+      </c>
+      <c r="AM24">
+        <v>151.758552352408</v>
+      </c>
+      <c r="AN24">
+        <v>134.84679129158599</v>
+      </c>
+      <c r="AO24">
+        <v>255.399911261668</v>
+      </c>
+      <c r="AP24">
+        <v>203.35855179665899</v>
+      </c>
       <c r="AQ24" s="5">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AR24" s="2"/>
-      <c r="AS24" s="3"/>
-      <c r="AT24" s="3"/>
-      <c r="AU24" s="3"/>
-      <c r="AV24" s="3"/>
+        <v>972.85751284575792</v>
+      </c>
+      <c r="AR24">
+        <v>7.8517853260040198</v>
+      </c>
+      <c r="AS24">
+        <v>7.49700832366943</v>
+      </c>
+      <c r="AT24">
+        <v>6.1034948348998999</v>
+      </c>
+      <c r="AU24">
+        <v>68.325308823585502</v>
+      </c>
+      <c r="AV24">
+        <v>5.7863674640655498</v>
+      </c>
       <c r="AW24" s="3">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>95.563964772224395</v>
       </c>
       <c r="AX24" s="2"/>
       <c r="AY24" s="3"/>
@@ -4604,23 +5287,43 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AL25" s="2"/>
-      <c r="AM25" s="3"/>
-      <c r="AN25" s="3"/>
-      <c r="AO25" s="3"/>
-      <c r="AP25" s="3"/>
+      <c r="AL25" s="2">
+        <v>313.13217148424201</v>
+      </c>
+      <c r="AM25">
+        <v>153.274802852101</v>
+      </c>
+      <c r="AN25">
+        <v>241.67154979377401</v>
+      </c>
+      <c r="AO25">
+        <v>186.905239211657</v>
+      </c>
+      <c r="AP25">
+        <v>115.566897157905</v>
+      </c>
       <c r="AQ25" s="5">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AR25" s="2"/>
-      <c r="AS25" s="3"/>
-      <c r="AT25" s="3"/>
-      <c r="AU25" s="3"/>
-      <c r="AV25" s="3"/>
+        <v>1010.550660499679</v>
+      </c>
+      <c r="AR25">
+        <v>6.3835042715072596</v>
+      </c>
+      <c r="AS25">
+        <v>5.5008460044860801</v>
+      </c>
+      <c r="AT25">
+        <v>7.4261198520660399</v>
+      </c>
+      <c r="AU25">
+        <v>5.9573056459426796</v>
+      </c>
+      <c r="AV25">
+        <v>1.7914657831192</v>
+      </c>
       <c r="AW25" s="3">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>27.059241557121258</v>
       </c>
       <c r="AX25" s="2"/>
       <c r="AY25" s="3"/>
@@ -4732,7 +5435,7 @@
         <f t="shared" si="4"/>
         <v>22.824234175681962</v>
       </c>
-      <c r="Z26">
+      <c r="Z26" s="2">
         <v>207.76084254760599</v>
       </c>
       <c r="AA26">
@@ -4770,7 +5473,7 @@
         <f t="shared" si="6"/>
         <v>28.980239009857087</v>
       </c>
-      <c r="AL26">
+      <c r="AL26" s="2">
         <v>217.199137022526</v>
       </c>
       <c r="AM26">
@@ -4956,6 +5659,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="AL27" s="2"/>
       <c r="AQ27" s="5">
         <f t="shared" si="11"/>
         <v>0</v>

</xml_diff>